<commit_message>
User Mobility Project: - edit fuctionality implemented - re organized codes - added new constants file
</commit_message>
<xml_diff>
--- a/Checkpoint_User_Mobility/config/User-Mobility-Test.xlsx
+++ b/Checkpoint_User_Mobility/config/User-Mobility-Test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_User_Mobility\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_User_Mobility\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C200435F-B207-4C24-AC50-97AFFE56BE4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CE2FB3-6237-48DB-AC5F-FE3E26128E99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>User Email</t>
   </si>
@@ -33,16 +33,16 @@
     <t>Groups</t>
   </si>
   <si>
-    <t>kgeerdhary@auchan.com</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
-    <t>mhemaraju@auchan.com</t>
-  </si>
-  <si>
-    <t>delete</t>
+    <t>prd-auchan</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>dtrump@auchan.com</t>
   </si>
 </sst>
 </file>
@@ -424,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{858A042F-E78E-42AB-85EA-A4FEB9F441DE}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,29 +447,33 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{7C204F65-3DA0-4A96-B650-E75F8C5E34EE}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{CC3477BC-D85C-48D0-9C39-A00340EA6BCE}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{CE16F144-3E31-4674-8429-DBC2F5951C10}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User Mobility Project: - Logging function implemented - After publishing the session, the scrippt will install the policy too - utils.py added for logger function
</commit_message>
<xml_diff>
--- a/Checkpoint_User_Mobility/config/User-Mobility-Test.xlsx
+++ b/Checkpoint_User_Mobility/config/User-Mobility-Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\My Projects\Python Projects\Github\Checkpoint_Automation\Checkpoint_User_Mobility\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CE2FB3-6237-48DB-AC5F-FE3E26128E99}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD51E9A8-1ABA-4532-B8D4-7D40A5599E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
+    <workbookView xWindow="3552" yWindow="3324" windowWidth="15132" windowHeight="7980" xr2:uid="{16F75F55-80E2-4A16-9DAD-18C417E0A39C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>User Email</t>
   </si>
@@ -36,13 +36,31 @@
     <t>Action</t>
   </si>
   <si>
+    <t>rislam@auchan.com</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>add</t>
+  </si>
+  <si>
+    <t>group-1;group2</t>
+  </si>
+  <si>
+    <t>foozeer@auchan.com</t>
+  </si>
+  <si>
+    <t>kgeerdharry@auchan.com</t>
+  </si>
+  <si>
+    <t>telephone@auchan.com</t>
+  </si>
+  <si>
     <t>prd-auchan</t>
   </si>
   <si>
-    <t>add</t>
-  </si>
-  <si>
-    <t>dtrump@auchan.com</t>
+    <t>edit</t>
   </si>
 </sst>
 </file>
@@ -427,7 +445,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,28 +470,48 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{CE16F144-3E31-4674-8429-DBC2F5951C10}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{65149EB1-CE65-4FC2-9B50-80B87A676724}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{3EBD452D-0665-48B7-89DD-131AE2C9F1E5}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{AFE061DD-B172-4F67-8BF2-22C3F8659459}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{8DEA0D80-1AE7-4E0E-BC2F-492C29B4572F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>